<commit_message>
- support formula evaluation after inserting the data - logs
</commit_message>
<xml_diff>
--- a/OUTPUT/excel/exel.xlsx
+++ b/OUTPUT/excel/exel.xlsx
@@ -9,17 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data-source" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,7 +334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
@@ -345,4 +342,25 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <f>'data-source'!C2</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>